<commit_message>
Update template files, add delay after upload file
</commit_message>
<xml_diff>
--- a/Testcase Generate from Gitlab/input/Testcase-template-erp-server.xlsx
+++ b/Testcase Generate from Gitlab/input/Testcase-template-erp-server.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7190"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7190" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="7" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Test Case Description</t>
   </si>
@@ -97,6 +98,24 @@
   </si>
   <si>
     <t>Response success, return with token</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>https://xm.iptp.dev/xm/api/channelmembers</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POST </t>
+  </si>
+  <si>
+    <t>Response</t>
+  </si>
+  <si>
+    <t>Request Body</t>
   </si>
 </sst>
 </file>
@@ -106,7 +125,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmmm\ d\,\ yyyy"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -152,6 +171,12 @@
       <u/>
       <sz val="10"/>
       <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -287,7 +312,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -323,12 +348,25 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -337,6 +375,69 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -360,85 +461,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -745,7 +772,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
@@ -757,50 +784,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="26"/>
+      <c r="B1" s="33"/>
       <c r="C1" s="1">
         <v>43</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="26"/>
-      <c r="F1" s="16" t="s">
+      <c r="E1" s="33"/>
+      <c r="F1" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="17"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="22"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="26"/>
+      <c r="B2" s="33"/>
       <c r="C2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="26"/>
-      <c r="F2" s="16" t="s">
+      <c r="E2" s="33"/>
+      <c r="F2" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="17"/>
-      <c r="H2" s="33" t="s">
+      <c r="G2" s="22"/>
+      <c r="H2" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="26"/>
-      <c r="J2" s="34" t="s">
+      <c r="I2" s="33"/>
+      <c r="J2" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="35"/>
+      <c r="K2" s="36"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
@@ -816,10 +843,10 @@
       <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="37"/>
+      <c r="B4" s="38"/>
       <c r="C4" s="10"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -844,31 +871,31 @@
       <c r="K5" s="4"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="37"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="37"/>
-      <c r="F6" s="38">
+      <c r="E6" s="38"/>
+      <c r="F6" s="39">
         <f ca="1">TODAY()</f>
         <v>44999</v>
       </c>
-      <c r="G6" s="39"/>
-      <c r="H6" s="33" t="s">
+      <c r="G6" s="40"/>
+      <c r="H6" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="37"/>
-      <c r="J6" s="32" t="str">
+      <c r="I6" s="38"/>
+      <c r="J6" s="31" t="str">
         <f>IF(COUNTIF(I18:I34,"Fail")&gt;0, "Fail", "Pass")</f>
         <v>Pass</v>
       </c>
-      <c r="K6" s="32"/>
+      <c r="K6" s="31"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
@@ -887,86 +914,86 @@
       <c r="A8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
       <c r="E8" s="7"/>
       <c r="F8" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="30" t="s">
+      <c r="G8" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
     </row>
     <row r="9" spans="1:11" ht="13" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8">
         <v>1</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="20"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="46"/>
       <c r="E9" s="3"/>
       <c r="F9" s="8">
         <v>1</v>
       </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="17"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="22"/>
     </row>
     <row r="10" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="8">
         <v>2</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="20"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="46"/>
       <c r="E10" s="3"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="17"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="22"/>
     </row>
     <row r="11" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="8">
         <v>3</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="20"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="46"/>
       <c r="E11" s="3"/>
       <c r="F11" s="8"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="17"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="22"/>
     </row>
     <row r="12" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="8">
         <v>4</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="20"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="46"/>
       <c r="E12" s="3"/>
       <c r="F12" s="8"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="17"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="22"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
@@ -997,146 +1024,149 @@
       <c r="K14" s="4"/>
     </row>
     <row r="16" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="24" t="s">
+      <c r="C16" s="48"/>
+      <c r="D16" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="25"/>
-      <c r="F16" s="21" t="s">
+      <c r="E16" s="51"/>
+      <c r="F16" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="21" t="s">
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="J16" s="27"/>
-      <c r="K16" s="27"/>
+      <c r="J16" s="52"/>
+      <c r="K16" s="52"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="22"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="27"/>
+      <c r="A17" s="48"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="52"/>
     </row>
     <row r="18" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8">
         <v>1</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="17"/>
-      <c r="D18" s="15" t="s">
+      <c r="C18" s="22"/>
+      <c r="D18" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="17"/>
-      <c r="F18" s="15" t="s">
+      <c r="E18" s="22"/>
+      <c r="F18" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="16"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="15" t="s">
+      <c r="G18" s="21"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="J18" s="16"/>
-      <c r="K18" s="17"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="22"/>
     </row>
     <row r="19" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8">
         <f>A18+1</f>
         <v>2</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="41"/>
-      <c r="H19" s="42"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="17"/>
-    </row>
-    <row r="20" spans="1:11" s="52" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="43">
+      <c r="B19" s="15"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="22"/>
+    </row>
+    <row r="20" spans="1:11" s="14" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="13">
         <f t="shared" ref="A20:A22" si="0">A19+1</f>
         <v>3</v>
       </c>
-      <c r="B20" s="44"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="44"/>
-      <c r="E20" s="44"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="47"/>
-      <c r="H20" s="48"/>
-      <c r="I20" s="49"/>
-      <c r="J20" s="50"/>
-      <c r="K20" s="51"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="30"/>
     </row>
     <row r="21" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="41"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="17"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="22"/>
     </row>
     <row r="22" spans="1:11" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B22" s="13"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="41"/>
-      <c r="H22" s="42"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="17"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:C17"/>
+    <mergeCell ref="D16:E17"/>
+    <mergeCell ref="F16:H17"/>
+    <mergeCell ref="I16:K17"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="G10:K10"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
@@ -1151,25 +1181,22 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="G10:K10"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:C17"/>
-    <mergeCell ref="D16:E17"/>
-    <mergeCell ref="F16:H17"/>
-    <mergeCell ref="I16:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="G11:K11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="G12:K12"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:K22"/>
   </mergeCells>
   <conditionalFormatting sqref="J6:K6">
     <cfRule type="expression" dxfId="2" priority="2">
@@ -1188,4 +1215,46 @@
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+      <c r="A1" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="54" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+      <c r="A2" s="53" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+      <c r="A3" s="53" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="53" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Make General report to collapse all report to 1 file
</commit_message>
<xml_diff>
--- a/Testcase Generate from Gitlab/input/Testcase-template-erp-server.xlsx
+++ b/Testcase Generate from Gitlab/input/Testcase-template-erp-server.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7190" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7190"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t>Test Case Description</t>
   </si>
@@ -116,6 +116,12 @@
   </si>
   <si>
     <t>Request Body</t>
+  </si>
+  <si>
+    <t>ERP user/ pass: superuser/ superuser</t>
+  </si>
+  <si>
+    <t>ERP user/ pass: phuong/ superuser</t>
   </si>
 </sst>
 </file>
@@ -352,92 +358,16 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -461,11 +391,87 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -772,8 +778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9:K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -787,47 +793,47 @@
       <c r="A1" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="33"/>
+      <c r="B1" s="28"/>
       <c r="C1" s="1">
         <v>43</v>
       </c>
       <c r="D1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="33"/>
-      <c r="F1" s="21" t="s">
+      <c r="E1" s="28"/>
+      <c r="F1" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="22"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="18"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="33"/>
+      <c r="B2" s="28"/>
       <c r="C2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="33"/>
-      <c r="F2" s="21" t="s">
+      <c r="E2" s="28"/>
+      <c r="F2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="22"/>
-      <c r="H2" s="34" t="s">
+      <c r="G2" s="18"/>
+      <c r="H2" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="33"/>
-      <c r="J2" s="35" t="s">
+      <c r="I2" s="28"/>
+      <c r="J2" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="36"/>
+      <c r="K2" s="37"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
@@ -843,10 +849,10 @@
       <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="38"/>
+      <c r="B4" s="39"/>
       <c r="C4" s="10"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -871,31 +877,31 @@
       <c r="K5" s="4"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="38"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="38"/>
-      <c r="F6" s="39">
+      <c r="E6" s="39"/>
+      <c r="F6" s="40">
         <f ca="1">TODAY()</f>
-        <v>44999</v>
-      </c>
-      <c r="G6" s="40"/>
-      <c r="H6" s="34" t="s">
+        <v>45000</v>
+      </c>
+      <c r="G6" s="41"/>
+      <c r="H6" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="38"/>
-      <c r="J6" s="31" t="str">
+      <c r="I6" s="39"/>
+      <c r="J6" s="34" t="str">
         <f>IF(COUNTIF(I18:I34,"Fail")&gt;0, "Fail", "Pass")</f>
         <v>Pass</v>
       </c>
-      <c r="K6" s="31"/>
+      <c r="K6" s="34"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
@@ -914,11 +920,11 @@
       <c r="A8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
       <c r="E8" s="7"/>
       <c r="F8" s="12" t="s">
         <v>8</v>
@@ -926,74 +932,80 @@
       <c r="G8" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="43"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
     </row>
     <row r="9" spans="1:11" ht="13" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8">
         <v>1</v>
       </c>
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="45"/>
-      <c r="D9" s="46"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="22"/>
       <c r="E9" s="3"/>
       <c r="F9" s="8">
         <v>1</v>
       </c>
-      <c r="G9" s="20"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="22"/>
+      <c r="G9" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="18"/>
     </row>
     <row r="10" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="8">
         <v>2</v>
       </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="46"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="22"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="22"/>
+      <c r="F10" s="8">
+        <v>2</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="18"/>
     </row>
     <row r="11" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="8">
         <v>3</v>
       </c>
-      <c r="B11" s="44"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="46"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="22"/>
       <c r="E11" s="3"/>
       <c r="F11" s="8"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="22"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="18"/>
     </row>
     <row r="12" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="8">
         <v>4</v>
       </c>
-      <c r="B12" s="44"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="46"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="22"/>
       <c r="E12" s="3"/>
       <c r="F12" s="8"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="22"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="18"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
@@ -1024,149 +1036,146 @@
       <c r="K14" s="4"/>
     </row>
     <row r="16" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="47" t="s">
+      <c r="B16" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="48"/>
-      <c r="D16" s="50" t="s">
+      <c r="C16" s="24"/>
+      <c r="D16" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="51"/>
-      <c r="F16" s="47" t="s">
+      <c r="E16" s="27"/>
+      <c r="F16" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="52"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="47" t="s">
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="J16" s="52"/>
-      <c r="K16" s="52"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="48"/>
-      <c r="B17" s="49"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="52"/>
-      <c r="I17" s="52"/>
-      <c r="J17" s="52"/>
-      <c r="K17" s="52"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
     </row>
     <row r="18" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8">
         <v>1</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="22"/>
-      <c r="D18" s="20" t="s">
+      <c r="C18" s="18"/>
+      <c r="D18" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="22"/>
-      <c r="F18" s="20" t="s">
+      <c r="E18" s="18"/>
+      <c r="F18" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="21"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="20" t="s">
+      <c r="G18" s="19"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="J18" s="21"/>
-      <c r="K18" s="22"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="18"/>
     </row>
     <row r="19" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8">
         <f>A18+1</f>
         <v>2</v>
       </c>
-      <c r="B19" s="15"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="21"/>
-      <c r="K19" s="22"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="18"/>
     </row>
     <row r="20" spans="1:11" s="14" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13">
         <f t="shared" ref="A20:A22" si="0">A19+1</f>
         <v>3</v>
       </c>
-      <c r="B20" s="23"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="29"/>
-      <c r="K20" s="30"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="50"/>
+      <c r="H20" s="51"/>
+      <c r="I20" s="52"/>
+      <c r="J20" s="53"/>
+      <c r="K20" s="54"/>
     </row>
     <row r="21" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B21" s="15"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="22"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="18"/>
     </row>
     <row r="22" spans="1:11" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="22"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="G11:K11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="G12:K12"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:C17"/>
-    <mergeCell ref="D16:E17"/>
-    <mergeCell ref="F16:H17"/>
-    <mergeCell ref="I16:K17"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="G10:K10"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I20:K20"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
@@ -1181,22 +1190,25 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="G10:K10"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:C17"/>
+    <mergeCell ref="D16:E17"/>
+    <mergeCell ref="F16:H17"/>
+    <mergeCell ref="I16:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="I18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="J6:K6">
     <cfRule type="expression" dxfId="2" priority="2">
@@ -1221,22 +1233,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="16" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="13" x14ac:dyDescent="0.3">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="15" t="s">
         <v>28</v>
       </c>
       <c r="B2" t="s">
@@ -1244,10 +1256,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="13" x14ac:dyDescent="0.3">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="53" t="s">
+      <c r="I3" s="15" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>